<commit_message>
deleção de historico r
</commit_message>
<xml_diff>
--- a/hemocentro/dados_sangue.xlsx
+++ b/hemocentro/dados_sangue.xlsx
@@ -10,9 +10,6 @@
     <sheet name="total" sheetId="1" r:id="rId1"/>
     <sheet name="aferese" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="Bolsas">total!$A$1</definedName>
-  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -984,10 +981,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A115"/>
+  <dimension ref="A1:A108"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -1531,27 +1528,6 @@
       <c r="A108" s="5">
         <v>4372</v>
       </c>
-    </row>
-    <row r="109" ht="15" spans="1:1">
-      <c r="A109" s="4"/>
-    </row>
-    <row r="110" ht="15" spans="1:1">
-      <c r="A110" s="4"/>
-    </row>
-    <row r="111" ht="15" spans="1:1">
-      <c r="A111" s="4"/>
-    </row>
-    <row r="112" ht="15" spans="1:1">
-      <c r="A112" s="4"/>
-    </row>
-    <row r="113" ht="15" spans="1:1">
-      <c r="A113" s="4"/>
-    </row>
-    <row r="114" ht="15" spans="1:1">
-      <c r="A114" s="4"/>
-    </row>
-    <row r="115" ht="15" spans="1:1">
-      <c r="A115" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1564,8 +1540,8 @@
   <sheetPr/>
   <dimension ref="A1:A108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>

</xml_diff>